<commit_message>
OKURWA WSZYSTKIE U_B SA ZLE XDDDDDDDDD
</commit_message>
<xml_diff>
--- a/Spraw2/lab2.xlsx
+++ b/Spraw2/lab2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3B4DB9-E0EA-487C-A687-BA2B3AA7732B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33408210-5954-4E94-8C27-2D2C632EE251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,9 +130,6 @@
     <t>RO_C Gliceryny=</t>
   </si>
   <si>
-    <t>Blad:</t>
-  </si>
-  <si>
     <t>Jednostka</t>
   </si>
   <si>
@@ -176,6 +173,9 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Niep.:</t>
   </si>
 </sst>
 </file>
@@ -678,49 +678,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="11">
         <v>0.34100000000000003</v>
@@ -732,7 +732,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>26</v>
       </c>
@@ -758,7 +758,7 @@
         <v>5</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>6</v>
@@ -785,7 +785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>27</v>
       </c>
@@ -838,7 +838,7 @@
         <v>37.08</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>28</v>
       </c>
@@ -891,7 +891,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>29</v>
       </c>
@@ -944,7 +944,7 @@
         <v>37.159999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>33</v>
       </c>
@@ -997,7 +997,7 @@
         <v>37.92</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F8" s="2">
         <v>5</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>37.39</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F9" s="2">
         <v>6</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="13"/>
       <c r="F10" s="2">
         <v>7</v>
@@ -1121,13 +1121,13 @@
         <v>36.86</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="13">
         <f>SQRT((6/(3.14159*G27^3))^2*0.00000001^2+((18*L27)/(3.13159*G27^4))^2*J27^2)</f>
         <v>685.2268695948502</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F11" s="2">
         <v>8</v>
@@ -1169,13 +1169,13 @@
         <v>37.39</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="13">
         <f>SQRT((6/(3.14159*H27^3))^2*0.00000001^2+((18*M27)/(3.13159*H27^4))^2*J27^2)</f>
         <v>1069.6997763292379</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="2">
         <v>9</v>
@@ -1217,13 +1217,13 @@
         <v>36.520000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <f>SQRT((6/(3.14159*I27^3))^2*0.00000001^2+((18*N27)/(3.13159*I27^4))^2*J27^2)</f>
         <v>574.11430895963281</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2">
         <v>10</v>
@@ -1265,7 +1265,7 @@
         <v>36.29</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="F16" s="9" t="s">
         <v>12</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F17" s="9">
         <f>F4</f>
         <v>1</v>
@@ -1358,7 +1358,7 @@
         <v>37.08</v>
       </c>
     </row>
-    <row r="18" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F18" s="9">
         <f t="shared" ref="F18:F26" si="2">F5</f>
         <v>2</v>
@@ -1410,7 +1410,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F19" s="9">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -1462,7 +1462,7 @@
         <v>37.159999999999997</v>
       </c>
     </row>
-    <row r="20" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F20" s="9">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -1514,7 +1514,7 @@
         <v>37.92</v>
       </c>
     </row>
-    <row r="21" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F21" s="9">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -1566,7 +1566,7 @@
         <v>37.39</v>
       </c>
     </row>
-    <row r="22" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F22" s="9">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -1618,7 +1618,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="23" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F23" s="9">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1670,7 +1670,7 @@
         <v>36.86</v>
       </c>
     </row>
-    <row r="24" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F24" s="9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1722,7 +1722,7 @@
         <v>37.39</v>
       </c>
     </row>
-    <row r="25" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F25" s="9">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1774,7 +1774,7 @@
         <v>36.520000000000003</v>
       </c>
     </row>
-    <row r="26" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F26" s="9">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1826,7 +1826,7 @@
         <v>36.29</v>
       </c>
     </row>
-    <row r="27" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:21" x14ac:dyDescent="0.3">
       <c r="F27" t="s">
         <v>24</v>
       </c>
@@ -1877,27 +1877,27 @@
         <v>37.041000000000004</v>
       </c>
     </row>
-    <row r="28" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:21" x14ac:dyDescent="0.3">
       <c r="P28" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>37</v>
+      </c>
+      <c r="R28" t="s">
         <v>38</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="S28" t="s">
         <v>38</v>
       </c>
-      <c r="R28" t="s">
-        <v>39</v>
-      </c>
-      <c r="S28" t="s">
-        <v>39</v>
-      </c>
       <c r="T28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="6:21" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="6:21" x14ac:dyDescent="0.3">
       <c r="P29">
         <f>P17-$P$27</f>
         <v>1.4000000000002899E-2</v>
@@ -1923,7 +1923,7 @@
         <v>1.5209999999995611E-3</v>
       </c>
     </row>
-    <row r="30" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:21" x14ac:dyDescent="0.3">
       <c r="P30">
         <f t="shared" ref="P30:P38" si="12">P18-$P$27</f>
         <v>-0.11599999999999611</v>
@@ -1949,7 +1949,7 @@
         <v>1.6810000000003216E-3</v>
       </c>
     </row>
-    <row r="31" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:21" x14ac:dyDescent="0.3">
       <c r="P31">
         <f t="shared" si="12"/>
         <v>1.7640000000000029</v>
@@ -1975,7 +1975,7 @@
         <v>1.4160999999998255E-2</v>
       </c>
     </row>
-    <row r="32" spans="6:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:21" x14ac:dyDescent="0.3">
       <c r="P32">
         <f t="shared" si="12"/>
         <v>-0.41599999999999682</v>
@@ -2001,7 +2001,7 @@
         <v>0.77264099999999614</v>
       </c>
     </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
       <c r="P33">
         <f t="shared" si="12"/>
         <v>-0.45599999999999596</v>
@@ -2027,22 +2027,22 @@
         <v>0.12180099999999766</v>
       </c>
     </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D34">
         <f>SQRT((G27*B3*P27*(B4-B7)/(9*B2))^2*J27^2+(G27^2*B3*(B4-B7)/(18*B2))^2*Q42^2+(G27^2*B3*P27/(18*B2))^2*A11^2+(G27^2*B3*P27/(18*B2))^2*C7^2+(G27^2*B3*P27*(B4-B7)/(18*B2^2))^2*C2^2)</f>
         <v>1.3243623061148884</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P34">
         <f t="shared" si="12"/>
@@ -2069,9 +2069,9 @@
         <v>5.8081000000003262E-2</v>
       </c>
     </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35">
         <f>SQRT((H27*B3*Q27*(B5-B7)/(9*B2))^2*J27^2+(H27^2*B3*(B5-B7)/(18*B2))^2*S42^2+(H27^2*B3*Q27/(18*B2))^2*A12^2+(H27^2*B3*Q27/(18*B2))^2*C7^2+(H27^2*B3*Q27*(B5-B7)/(18*B2^2))^2*C2^2)</f>
@@ -2106,9 +2106,9 @@
         <v>3.2761000000001622E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36">
         <f>SQRT((I27*B3*R27*(B6-B7)/(9*B2))^2*J27^2+(I27^2*B3*(B6-B7)/(18*B2))^2*U42^2+(I27^2*B3*R27/(18*B2))^2*A13^2+(I27^2*B3*R27/(18*B2))^2*C7^2+(I27^2*B3*R27*(B6-B7)/(18*B2^2))^2*C2^2)</f>
@@ -2139,7 +2139,7 @@
         <v>0.12180099999999766</v>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:21" x14ac:dyDescent="0.3">
       <c r="P37">
         <f t="shared" si="12"/>
         <v>-0.34599999999999653</v>
@@ -2165,7 +2165,7 @@
         <v>0.27144100000000082</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:21" x14ac:dyDescent="0.3">
       <c r="P38">
         <f t="shared" si="12"/>
         <v>-9.5999999999996533E-2</v>
@@ -2191,23 +2191,23 @@
         <v>0.56400100000000719</v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39">
         <v>0.93479999999999996</v>
       </c>
       <c r="F39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D40">
         <v>0.99839999999999995</v>
@@ -2217,7 +2217,7 @@
         <v>0.89206666666666656</v>
       </c>
       <c r="P40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q40">
         <f>SQRT(SUM(Q29:Q38)/(90))</f>
@@ -2232,17 +2232,17 @@
         <v>0.14756881633853267</v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D41">
         <v>0.74299999999999999</v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:21" x14ac:dyDescent="0.3">
       <c r="P42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q42">
         <f>SQRT(Q40^2+0.02^2/3)</f>

</xml_diff>